<commit_message>
Update player data, activity logs, and war records; add new input files and adjust strike details
</commit_message>
<xml_diff>
--- a/war_bases.xlsx
+++ b/war_bases.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
   <si>
     <t>Number</t>
   </si>
@@ -43,97 +43,97 @@
     <t>War 7</t>
   </si>
   <si>
-    <t>Hallow Hero</t>
-  </si>
-  <si>
     <t>Satan</t>
   </si>
   <si>
+    <t>fwa</t>
+  </si>
+  <si>
     <t>Kaselcap</t>
   </si>
   <si>
+    <t>BumblinMumbler</t>
+  </si>
+  <si>
     <t>Sned</t>
   </si>
   <si>
-    <t>ViperX56</t>
-  </si>
-  <si>
     <t>Smitty™</t>
   </si>
   <si>
-    <t>ANBU</t>
-  </si>
-  <si>
-    <t>fwa</t>
-  </si>
-  <si>
     <t>Protips</t>
   </si>
   <si>
-    <t>jy</t>
-  </si>
-  <si>
     <t>katsu</t>
   </si>
   <si>
     <t>pg</t>
   </si>
   <si>
-    <t>W1nter</t>
-  </si>
-  <si>
-    <t>Cmdn</t>
+    <t>Big Daddy T</t>
+  </si>
+  <si>
+    <t>Vojt</t>
+  </si>
+  <si>
+    <t>K.L.A.U.S</t>
+  </si>
+  <si>
+    <t>Anas</t>
+  </si>
+  <si>
+    <t>Az7777</t>
   </si>
   <si>
     <t>Hadez</t>
   </si>
   <si>
-    <t>slothnz</t>
-  </si>
-  <si>
-    <t>jwong</t>
+    <t>Ascended</t>
+  </si>
+  <si>
+    <t>Baleus</t>
+  </si>
+  <si>
+    <t>YouAreMyBreh</t>
   </si>
   <si>
     <t>Rod</t>
   </si>
   <si>
-    <t>skyeshade</t>
-  </si>
-  <si>
-    <t>Baleus</t>
-  </si>
-  <si>
-    <t>phr*</t>
-  </si>
-  <si>
-    <t>Ascended</t>
-  </si>
-  <si>
-    <t>Narrowl</t>
-  </si>
-  <si>
-    <t>DPK|LLZONE</t>
-  </si>
-  <si>
-    <t>YouAreMyBreh</t>
-  </si>
-  <si>
-    <t>your mama</t>
+    <t>xHead_Bangerx</t>
+  </si>
+  <si>
+    <t>Mythos</t>
+  </si>
+  <si>
+    <t>Plantos</t>
   </si>
   <si>
     <t>ImagineWaggons</t>
   </si>
   <si>
-    <t>Ligma</t>
+    <t>Luke</t>
+  </si>
+  <si>
+    <t>shadow</t>
+  </si>
+  <si>
+    <t>Welli</t>
+  </si>
+  <si>
+    <t>Motz</t>
+  </si>
+  <si>
+    <t>LOGAN911</t>
+  </si>
+  <si>
+    <t>potatoes</t>
   </si>
   <si>
     <t>DNG</t>
   </si>
   <si>
-    <t>Mythos</t>
-  </si>
-  <si>
-    <t>Plantos</t>
+    <t>Asrar</t>
   </si>
 </sst>
 </file>
@@ -457,20 +457,34 @@
       </c>
       <c r="C2" s="3">
         <f t="shared" ref="C2:C31" si="1">COUNTA(D2:J2)</f>
-        <v>0</v>
-      </c>
-      <c r="D2" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
     </row>
     <row r="3">
       <c r="A3" s="2">
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4">
@@ -478,7 +492,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" si="1"/>
@@ -490,7 +504,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" si="1"/>
@@ -502,7 +516,7 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" si="1"/>
@@ -514,7 +528,7 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" si="1"/>
@@ -526,17 +540,11 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -548,10 +556,7 @@
       </c>
       <c r="C9" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -563,28 +568,10 @@
       </c>
       <c r="C10" s="3">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11">
@@ -610,6 +597,13 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
     </row>
     <row r="13">
       <c r="A13" s="2">
@@ -622,13 +616,6 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
     </row>
     <row r="14">
       <c r="A14" s="2">
@@ -639,13 +626,7 @@
       </c>
       <c r="C14" s="3">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -700,10 +681,13 @@
       </c>
       <c r="C18" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="19">
@@ -729,13 +713,6 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
     </row>
     <row r="21">
       <c r="A21" s="2">
@@ -746,8 +723,19 @@
       </c>
       <c r="C21" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
     </row>
     <row r="22">
       <c r="A22" s="2">
@@ -770,28 +758,7 @@
       </c>
       <c r="C23" s="3">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -803,10 +770,7 @@
       </c>
       <c r="C24" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -830,10 +794,7 @@
       </c>
       <c r="C26" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -857,7 +818,22 @@
       </c>
       <c r="C28" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="29">
@@ -893,28 +869,7 @@
       </c>
       <c r="C31" s="3">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>